<commit_message>
fix the test case
</commit_message>
<xml_diff>
--- a/src/app/app-playloader/data/sample.02.xlsx
+++ b/src/app/app-playloader/data/sample.02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joeylam/repo/njs/njstool/src/app/app-playloader/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489AEF78-8D58-E840-9D72-DC86DDA186F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E057428-22D0-2C46-B345-1D0084F8BC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" xr2:uid="{EA9BDBA2-0CC1-8A42-AB5A-3B400F638747}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Field</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>num</t>
+  </si>
+  <si>
+    <t>list.str</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,7 +547,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>8</v>

</xml_diff>